<commit_message>
Published state of ETDataset on March 11 2021
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy/energy_hydrogen_solar_pv_solar_radiation.central_producer.xlsx
+++ b/nodes_source_analyses/energy/energy/energy_hydrogen_solar_pv_solar_radiation.central_producer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/etdataset/nodes_source_analyses/energy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlottevonm/Code/etdataset/nodes_source_analyses/energy/energy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66C93F3-B821-BE4E-A4E2-42F720B377B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351D4A35-3BA3-2E4D-8B60-AFD622A13E38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="28340" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="762" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -45,7 +45,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -56,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="185">
   <si>
     <t>Source</t>
   </si>
@@ -642,9 +645,6 @@
     <t>m2/kW</t>
   </si>
   <si>
-    <t>PS. There is a mistake here that it should be 600 km2 instead of 600 m2</t>
-  </si>
-  <si>
     <t>area per kW</t>
   </si>
   <si>
@@ -775,6 +775,18 @@
   </si>
   <si>
     <t>See https://github.com/quintel/documentation/blob/master/general/cost_calculations.md#weighted-average-cost-of-capital</t>
+  </si>
+  <si>
+    <t>Zorg voor het landschap</t>
+  </si>
+  <si>
+    <t>PBL</t>
+  </si>
+  <si>
+    <t>https://refman.energytransitionmodel.com/publications/2138</t>
+  </si>
+  <si>
+    <t>https://www.pbl.nl/sites/default/files/downloads/pbl-2019-zorg-voor-landschap-3346_0.pdf</t>
   </si>
 </sst>
 </file>
@@ -782,14 +794,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
-    <numFmt numFmtId="169" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
+    <numFmt numFmtId="170" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="41">
     <font>
@@ -1714,10 +1726,10 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="40" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="40" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="219">
+  <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1786,22 +1798,22 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="2" fontId="24" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1829,7 +1841,7 @@
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
     <xf numFmtId="2" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
@@ -1856,11 +1868,11 @@
     <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="24" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1889,7 +1901,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="24" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1907,7 +1919,7 @@
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1919,13 +1931,13 @@
     <xf numFmtId="0" fontId="30" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1943,7 +1955,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="24" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1951,13 +1963,13 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1969,7 +1981,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="38" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1991,7 +2003,7 @@
     <xf numFmtId="2" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="24" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="38" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2020,21 +2032,21 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="177" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="24" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="2" borderId="22" xfId="308" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="22" xfId="308" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="3" fillId="2" borderId="22" xfId="308" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="22" xfId="308" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="6" borderId="22" xfId="308" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="3" fillId="6" borderId="22" xfId="308" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2044,7 +2056,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="3" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="3" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2059,7 +2071,7 @@
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="309" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2091,6 +2103,14 @@
     <xf numFmtId="0" fontId="38" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="177" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="310">
     <cellStyle name="Comma" xfId="308" builtinId="3"/>
@@ -2525,50 +2545,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1675531</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>172071</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="6531405" cy="4916698"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A26A38F9-2A87-A74A-8B38-1D827462F820}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="4644" t="15362" r="5319"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10768731" y="8312771"/>
-          <a:ext cx="6531405" cy="4916698"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -2596,7 +2572,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2646,7 +2622,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2696,7 +2672,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2740,7 +2716,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2784,7 +2760,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2828,7 +2804,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2843,6 +2819,114 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>169333</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>186267</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>181132</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>198967</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3525D203-D749-F940-A8B8-62BA3D1CA3C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8957733" y="5689600"/>
+          <a:ext cx="5701399" cy="4076700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>520699</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>135466</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Oval 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67A68507-FCE0-A44F-B244-89A0216CC5E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12153899" y="6671733"/>
+          <a:ext cx="2459567" cy="1032933"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3470,7 +3554,7 @@
   </sheetPr>
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -3841,7 +3925,7 @@
       </c>
       <c r="H22" s="30"/>
       <c r="I22" s="209" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J22" s="129"/>
     </row>
@@ -3948,7 +4032,7 @@
       </c>
       <c r="H27" s="30"/>
       <c r="I27" s="160" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J27" s="129"/>
     </row>
@@ -4005,7 +4089,7 @@
       </c>
       <c r="E31" s="99">
         <f>'Research data'!H12</f>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="F31" s="30"/>
       <c r="G31" s="30" t="s">
@@ -4394,7 +4478,7 @@
       </c>
       <c r="L3" s="120"/>
       <c r="M3" s="120" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N3" s="120"/>
       <c r="O3" s="120" t="s">
@@ -4590,13 +4674,13 @@
       <c r="G12" s="47"/>
       <c r="H12" s="55">
         <f>K12</f>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="I12" s="49"/>
       <c r="J12" s="49"/>
       <c r="K12" s="78">
         <f>Notes!E40</f>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="L12" s="32"/>
       <c r="M12" s="32"/>
@@ -4763,7 +4847,7 @@
     <row r="20" spans="2:15" ht="17" thickBot="1">
       <c r="B20" s="34"/>
       <c r="C20" s="205" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D20" s="58"/>
       <c r="E20" s="58"/>
@@ -4784,18 +4868,18 @@
       <c r="M20" s="32"/>
       <c r="N20" s="32"/>
       <c r="O20" s="208" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="17" thickBot="1">
       <c r="B21" s="34"/>
       <c r="C21" s="205" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D21" s="58"/>
       <c r="E21" s="58"/>
       <c r="F21" s="207" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G21" s="121"/>
       <c r="H21" s="50"/>
@@ -4933,8 +5017,8 @@
   </sheetPr>
   <dimension ref="B1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.140625" defaultRowHeight="16"/>
@@ -5151,10 +5235,10 @@
       </c>
       <c r="G16" s="180"/>
       <c r="H16" s="180" t="s">
+        <v>140</v>
+      </c>
+      <c r="I16" s="180" t="s">
         <v>141</v>
-      </c>
-      <c r="I16" s="180" t="s">
-        <v>142</v>
       </c>
       <c r="J16" s="96"/>
     </row>
@@ -5193,11 +5277,11 @@
     <row r="20" spans="2:10">
       <c r="B20" s="92"/>
       <c r="C20" s="180" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D20" s="180"/>
       <c r="E20" s="180" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F20" s="203">
         <v>2017</v>
@@ -5207,7 +5291,7 @@
         <v>2019</v>
       </c>
       <c r="I20" s="180" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J20" s="180"/>
     </row>
@@ -5220,20 +5304,36 @@
       <c r="G21" s="204"/>
       <c r="H21" s="180"/>
       <c r="I21" s="180" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J21" s="180"/>
     </row>
     <row r="22" spans="2:10">
       <c r="B22" s="92"/>
-      <c r="C22" s="180"/>
-      <c r="D22" s="180"/>
-      <c r="E22" s="180"/>
-      <c r="F22" s="203"/>
-      <c r="G22" s="198"/>
-      <c r="H22" s="180"/>
-      <c r="I22" s="180"/>
-      <c r="J22" s="180"/>
+      <c r="C22" s="219" t="s">
+        <v>181</v>
+      </c>
+      <c r="D22" s="219" t="s">
+        <v>182</v>
+      </c>
+      <c r="E22" s="219" t="s">
+        <v>171</v>
+      </c>
+      <c r="F22" s="220">
+        <v>2019</v>
+      </c>
+      <c r="G22" s="221">
+        <v>44242</v>
+      </c>
+      <c r="H22" s="219">
+        <v>2019</v>
+      </c>
+      <c r="I22" s="222" t="s">
+        <v>183</v>
+      </c>
+      <c r="J22" s="219" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="23" spans="2:10">
       <c r="B23" s="92"/>
@@ -5308,6 +5408,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H17" r:id="rId1" xr:uid="{D535C137-5B89-404E-9C2C-5EF152F0A141}"/>
+    <hyperlink ref="I22" r:id="rId2" xr:uid="{830F363C-BFA5-4443-90C3-7037939197D6}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5318,8 +5419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:V152"/>
   <sheetViews>
-    <sheetView topLeftCell="B103" workbookViewId="0">
-      <selection activeCell="D142" sqref="D142"/>
+    <sheetView topLeftCell="C20" zoomScale="131" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
@@ -5586,7 +5687,7 @@
     <row r="18" spans="2:14">
       <c r="B18" s="145"/>
       <c r="C18" s="183" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D18" s="137"/>
       <c r="E18" s="137"/>
@@ -5899,11 +6000,10 @@
     <row r="38" spans="2:22" s="180" customFormat="1">
       <c r="B38" s="185"/>
       <c r="D38" s="186" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E38" s="192">
-        <f>E35/(E34*1000)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F38" s="192" t="s">
         <v>136</v>
@@ -5919,11 +6019,11 @@
     <row r="39" spans="2:22" s="180" customFormat="1">
       <c r="B39" s="185"/>
       <c r="D39" s="186" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E39" s="193">
         <f>E38*E24</f>
-        <v>300000</v>
+        <v>200000</v>
       </c>
       <c r="F39" s="192" t="s">
         <v>99</v>
@@ -5939,11 +6039,11 @@
     <row r="40" spans="2:22" s="180" customFormat="1">
       <c r="B40" s="185"/>
       <c r="D40" s="186" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E40" s="194">
         <f>E39/1000000</f>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="F40" s="192" t="s">
         <v>4</v>
@@ -6120,9 +6220,7 @@
       <c r="E52" s="186"/>
       <c r="F52" s="186"/>
       <c r="G52" s="186"/>
-      <c r="I52" s="105" t="s">
-        <v>137</v>
-      </c>
+      <c r="I52" s="105"/>
       <c r="J52" s="183"/>
       <c r="K52" s="183"/>
       <c r="L52" s="183"/>
@@ -6173,7 +6271,7 @@
     <row r="56" spans="2:14">
       <c r="B56" s="145"/>
       <c r="C56" s="183" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D56" s="137"/>
       <c r="E56" s="137"/>
@@ -6248,7 +6346,7 @@
       <c r="B60" s="145"/>
       <c r="C60" s="137"/>
       <c r="D60" s="183" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E60" s="183">
         <f>AVERAGE(E58,E59)</f>
@@ -6402,7 +6500,7 @@
     <row r="70" spans="2:14">
       <c r="B70" s="145"/>
       <c r="C70" s="183" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D70" s="137"/>
       <c r="E70" s="137"/>
@@ -6420,10 +6518,10 @@
       <c r="B71" s="145"/>
       <c r="C71" s="137"/>
       <c r="D71" s="183" t="s">
+        <v>145</v>
+      </c>
+      <c r="E71" s="183" t="s">
         <v>146</v>
-      </c>
-      <c r="E71" s="183" t="s">
-        <v>147</v>
       </c>
       <c r="F71" s="137"/>
       <c r="G71" s="137"/>
@@ -6911,14 +7009,14 @@
       <c r="F103" s="186"/>
       <c r="G103" s="186"/>
       <c r="I103" s="186" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N103" s="187"/>
     </row>
     <row r="104" spans="2:14" s="180" customFormat="1">
       <c r="B104" s="185"/>
       <c r="C104" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D104" s="186"/>
       <c r="E104" s="186"/>
@@ -6933,21 +7031,21 @@
       <c r="F105" s="186"/>
       <c r="G105" s="186"/>
       <c r="K105" s="199" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L105" s="200">
         <f>0.83611</f>
         <v>0.83611000000000002</v>
       </c>
       <c r="M105" s="199" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N105" s="187"/>
     </row>
     <row r="106" spans="2:14" s="180" customFormat="1">
       <c r="B106" s="185"/>
       <c r="C106" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D106" s="186"/>
       <c r="E106" s="186"/>
@@ -6955,7 +7053,7 @@
       <c r="G106" s="186"/>
       <c r="K106" s="199"/>
       <c r="L106" s="201" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M106" s="199"/>
       <c r="N106" s="187"/>
@@ -7024,10 +7122,10 @@
     <row r="114" spans="2:14" s="180" customFormat="1">
       <c r="B114" s="185"/>
       <c r="C114" s="186" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D114" s="186" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E114" s="186"/>
       <c r="F114" s="186"/>
@@ -7039,13 +7137,13 @@
       <c r="C115" s="183"/>
       <c r="D115" s="186"/>
       <c r="E115" s="186" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F115" s="186">
         <v>871</v>
       </c>
       <c r="G115" s="186" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N115" s="187"/>
     </row>
@@ -7053,7 +7151,7 @@
       <c r="B116" s="185"/>
       <c r="C116" s="183"/>
       <c r="D116" s="186" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E116" s="186"/>
       <c r="F116" s="186"/>
@@ -7064,14 +7162,14 @@
       <c r="B117" s="185"/>
       <c r="C117" s="183"/>
       <c r="D117" s="186" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E117" s="186"/>
       <c r="F117" s="186">
         <v>440</v>
       </c>
       <c r="G117" s="186" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N117" s="187"/>
     </row>
@@ -7079,21 +7177,21 @@
       <c r="B118" s="185"/>
       <c r="C118" s="183"/>
       <c r="D118" s="186" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E118" s="186"/>
       <c r="F118" s="186">
         <v>84</v>
       </c>
       <c r="G118" s="186" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N118" s="187"/>
     </row>
     <row r="119" spans="2:14" s="180" customFormat="1">
       <c r="B119" s="185"/>
       <c r="D119" s="186" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E119" s="186"/>
       <c r="F119" s="186">
@@ -7101,28 +7199,28 @@
         <v>297</v>
       </c>
       <c r="G119" s="186" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N119" s="187"/>
     </row>
     <row r="120" spans="2:14" s="180" customFormat="1">
       <c r="B120" s="185"/>
       <c r="D120" s="186" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E120" s="206"/>
       <c r="F120" s="180">
         <v>50</v>
       </c>
       <c r="G120" s="186" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N120" s="187"/>
     </row>
     <row r="121" spans="2:14" s="180" customFormat="1">
       <c r="B121" s="185"/>
       <c r="F121" s="180" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N121" s="187"/>
     </row>
@@ -7145,13 +7243,13 @@
     <row r="124" spans="2:14" s="180" customFormat="1">
       <c r="B124" s="185"/>
       <c r="D124" s="186" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E124" s="186">
         <v>14.7</v>
       </c>
       <c r="F124" s="186" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G124" s="186"/>
       <c r="N124" s="187"/>
@@ -7161,7 +7259,7 @@
       <c r="D125" s="186"/>
       <c r="E125" s="186"/>
       <c r="F125" s="186" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G125" s="186"/>
       <c r="N125" s="187"/>
@@ -7169,13 +7267,13 @@
     <row r="126" spans="2:14" s="180" customFormat="1">
       <c r="B126" s="185"/>
       <c r="D126" s="186" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E126" s="186">
         <v>30</v>
       </c>
       <c r="G126" s="186" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N126" s="187"/>
     </row>
@@ -7190,14 +7288,14 @@
     <row r="128" spans="2:14" s="180" customFormat="1">
       <c r="B128" s="185"/>
       <c r="D128" s="186" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E128" s="186">
         <f>E124+(E126/E60)</f>
         <v>15.899999999999999</v>
       </c>
       <c r="F128" s="186" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G128" s="186"/>
       <c r="N128" s="187"/>
@@ -7306,7 +7404,7 @@
     <row r="141" spans="2:14">
       <c r="B141" s="145"/>
       <c r="D141" s="180" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N141" s="146"/>
     </row>

</xml_diff>